<commit_message>
added from last year
</commit_message>
<xml_diff>
--- a/DS_prev_year.xlsx
+++ b/DS_prev_year.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>אלמוג גל</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>מנסור מנסור</t>
+  </si>
+  <si>
+    <t>פתחאללה חאג'312319569</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -466,6 +469,17 @@
       </c>
       <c r="G5">
         <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>40.5</v>
+      </c>
+      <c r="G6">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>